<commit_message>
used: TypeMachine process finished
</commit_message>
<xml_diff>
--- a/04 - MID/01 - Create/03 - TypeMachine/Data_reTest.xlsx
+++ b/04 - MID/01 - Create/03 - TypeMachine/Data_reTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\04 - MID\01 - Create\03 - TypeMachine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDCACDB-2348-4A47-AA34-EF265A6F8049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CD3302-9747-4D6B-BE75-0DC8CFE492FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{3718D32B-9188-4ED9-B393-40F3181E94A9}"/>
   </bookViews>
@@ -39,14 +39,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Bico (normal final)</t>
   </si>
   <si>
-    <t>F000430904</t>
-  </si>
-  <si>
     <t>F002C40008</t>
   </si>
   <si>
@@ -75,6 +72,30 @@
   </si>
   <si>
     <t>04331727EW</t>
+  </si>
+  <si>
+    <t>F000430305</t>
+  </si>
+  <si>
+    <t>F000430311</t>
+  </si>
+  <si>
+    <t>F000430913</t>
+  </si>
+  <si>
+    <t>F000430914</t>
+  </si>
+  <si>
+    <t>F002C40902</t>
+  </si>
+  <si>
+    <t>H105025304</t>
+  </si>
+  <si>
+    <t>H105025420</t>
+  </si>
+  <si>
+    <t>H105025043</t>
   </si>
 </sst>
 </file>
@@ -164,10 +185,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -467,11 +484,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12FECC66-60F8-4D0C-9500-262A9824CD5F}">
-  <dimension ref="A1:A117"/>
+  <dimension ref="A1:A231"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -487,581 +502,1151 @@
     </row>
     <row r="2" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>433171284</v>
+        <v>433171012</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>433171964</v>
+        <v>433171080</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>433172234</v>
+        <v>433171082</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
+      <c r="A5" s="2">
+        <v>433171084</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>2</v>
+      <c r="A6" s="2">
+        <v>433171086</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>3</v>
+      <c r="A7" s="2">
+        <v>433171088</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>4</v>
+      <c r="A8" s="2">
+        <v>433171089</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>5</v>
+      <c r="A9" s="2">
+        <v>433171180</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
+      <c r="A10" s="2">
+        <v>433171182</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>7</v>
+      <c r="A11" s="2">
+        <v>433171183</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>8</v>
+      <c r="A12" s="2">
+        <v>433171185</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>9</v>
+      <c r="A13" s="2">
+        <v>433171186</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>10</v>
+      <c r="A14" s="2">
+        <v>433171187</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>11</v>
+      <c r="A15" s="2">
+        <v>433171188</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>433271180</v>
+        <v>433171189</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>433271481</v>
+        <v>433171254</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>433220184</v>
+        <v>433171280</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>433220185</v>
+        <v>433171281</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>433271780</v>
+        <v>433171282</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>433271286</v>
+        <v>433171284</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>433272980</v>
+        <v>433171285</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>433271685</v>
+        <v>433171286</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>433271680</v>
+        <v>433171287</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>433271785</v>
+        <v>433171288</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>433271883</v>
+        <v>433171289</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>433271886</v>
+        <v>433171344</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>433271280</v>
+        <v>433171385</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>433271482</v>
+        <v>433171386</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>433271480</v>
+        <v>433171387</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>433270088</v>
+        <v>433171388</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>433271589</v>
+        <v>433171462</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>433271784</v>
+        <v>433171482</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>433270181</v>
+        <v>433171484</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>433271688</v>
+        <v>433171485</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>433270089</v>
+        <v>433171487</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>433271086</v>
+        <v>433171562</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>433270084</v>
+        <v>433171581</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>433271686</v>
+        <v>433171582</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>433271884</v>
+        <v>433171584</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>433271486</v>
+        <v>433171585</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>433271487</v>
+        <v>433171586</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>433271588</v>
+        <v>433171587</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>433271683</v>
+        <v>433171680</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>433271587</v>
+        <v>433171684</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>433271284</v>
+        <v>433171685</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>433272987</v>
+        <v>433171686</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>433271684</v>
+        <v>433171687</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>433271681</v>
+        <v>433171688</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>433271682</v>
+        <v>433171689</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>433271687</v>
+        <v>433171780</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>433271783</v>
+        <v>433171781</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>433271788</v>
+        <v>433171782</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>433271789</v>
+        <v>433171784</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>433220087</v>
+        <v>433171786</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>433220089</v>
+        <v>433171787</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>433220180</v>
+        <v>433171789</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>433220182</v>
+        <v>433171812</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>433220183</v>
+        <v>433171844</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>433220186</v>
+        <v>433171881</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>433220187</v>
+        <v>433171882</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>433220189</v>
+        <v>433171964</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>433270081</v>
+        <v>433171985</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>433270082</v>
+        <v>433171986</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>433270085</v>
+        <v>433171987</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>433270180</v>
+        <v>433171988</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>433270183</v>
+        <v>433172011</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>433270185</v>
+        <v>433172083</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>433270186</v>
+        <v>433172085</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>433270187</v>
+        <v>433172086</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>433270188</v>
+        <v>433172161</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>433271081</v>
+        <v>433172234</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>433271087</v>
+        <v>433172271</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>433271183</v>
+        <v>433172387</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>433271184</v>
+        <v>433175081</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>433271186</v>
+        <v>433175086</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>433271281</v>
+        <v>433175087</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>433271282</v>
+        <v>433175088</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>433271285</v>
+        <v>433175089</v>
       </c>
     </row>
     <row r="80" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>433271287</v>
+        <v>433175180</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>433271289</v>
+        <v>433175185</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>433271380</v>
+        <v>433175186</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>433271381</v>
+        <v>433175189</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>433271383</v>
+        <v>433175271</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>433271384</v>
+        <v>433175280</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>433271385</v>
+        <v>433175285</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>433271388</v>
+        <v>433175324</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>433271389</v>
+        <v>433175383</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>433271485</v>
+        <v>433175384</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>433271488</v>
+        <v>433175385</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>433271489</v>
+        <v>433175386</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>433271580</v>
+        <v>433175387</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>433271581</v>
+        <v>433175389</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>433271582</v>
+        <v>433175390</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>433271583</v>
+        <v>433175404</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>433271584</v>
+        <v>433175449</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>433271585</v>
+        <v>433175453</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>433271586</v>
+        <v>433175472</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>433271781</v>
+        <v>433175480</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>433271782</v>
+        <v>433175481</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>433271787</v>
+        <v>433175482</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>433271882</v>
+        <v>433175483</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>433271885</v>
+        <v>433175484</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
-        <v>433271887</v>
+        <v>433175485</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
-        <v>433272985</v>
+        <v>433175486</v>
       </c>
     </row>
     <row r="106" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
-        <v>433272986</v>
+        <v>433175488</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
+        <v>433175489</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="2">
+        <v>433271180</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="2">
+        <v>433271481</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="2">
+        <v>433220184</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="2">
+        <v>433220185</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="2">
+        <v>433271780</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="2">
+        <v>433271286</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="2">
+        <v>433272980</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="2">
+        <v>433271685</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="2">
+        <v>433271680</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="2">
+        <v>433271785</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="2">
+        <v>433271883</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="2">
+        <v>433271886</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="2">
+        <v>433271280</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="2">
+        <v>433271482</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="2">
+        <v>433271480</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="2">
+        <v>433270088</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="2">
+        <v>433271589</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="2">
+        <v>433271784</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="2">
+        <v>433270181</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="2">
+        <v>433271688</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="2">
+        <v>433270089</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="2">
+        <v>433271086</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="2">
+        <v>433270084</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="2">
+        <v>433271686</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="2">
+        <v>433271884</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="2">
+        <v>433271486</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="2">
+        <v>433271487</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="2">
+        <v>433271588</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="2">
+        <v>433271683</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="2">
+        <v>433271587</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="2">
+        <v>433271284</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="2">
+        <v>433272987</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="2">
+        <v>433271684</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="2">
+        <v>433271681</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="2">
+        <v>433271682</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="2">
+        <v>433271687</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="2">
+        <v>433271783</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="2">
+        <v>433271788</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="2">
+        <v>433271789</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="2">
+        <v>433220087</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="2">
+        <v>433220089</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="2">
+        <v>433220180</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="2">
+        <v>433220182</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="2">
+        <v>433220183</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="2">
+        <v>433220186</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="2">
+        <v>433220187</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="2">
+        <v>433220189</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="2">
+        <v>433270081</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="2">
+        <v>433270082</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="2">
+        <v>433270085</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="2">
+        <v>433270180</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="2">
+        <v>433270183</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="2">
+        <v>433270185</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="2">
+        <v>433270186</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="2">
+        <v>433270187</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="2">
+        <v>433270188</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="2">
+        <v>433271081</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="2">
+        <v>433271087</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="2">
+        <v>433271183</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="2">
+        <v>433271184</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="2">
+        <v>433271186</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="2">
+        <v>433271281</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="2">
+        <v>433271282</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="2">
+        <v>433271285</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="2">
+        <v>433271287</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="2">
+        <v>433271289</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="2">
+        <v>433271380</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="2">
+        <v>433271381</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="2">
+        <v>433271383</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="2">
+        <v>433271384</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="2">
+        <v>433271385</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="2">
+        <v>433271388</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="2">
+        <v>433271389</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="2">
+        <v>433271485</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="2">
+        <v>433271488</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="2">
+        <v>433271489</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="2">
+        <v>433271501</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="2">
+        <v>433271580</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A203" s="2">
+        <v>433271581</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="2">
+        <v>433271582</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="2">
+        <v>433271583</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="2">
+        <v>433271584</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A207" s="2">
+        <v>433271585</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A208" s="2">
+        <v>433271586</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="2">
+        <v>433271622</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A210" s="2">
+        <v>433271762</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A211" s="2">
+        <v>433271781</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A212" s="2">
+        <v>433271782</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A213" s="2">
+        <v>433271787</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A214" s="2">
+        <v>433271882</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A215" s="2">
+        <v>433271885</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A216" s="2">
+        <v>433271887</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A217" s="2">
+        <v>433272985</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A218" s="2">
+        <v>433272986</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A219" s="2">
         <v>433272988</v>
       </c>
     </row>
-    <row r="108" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="2">
+    <row r="220" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A221" s="2">
         <v>433220081</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="2">
+    <row r="222" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A222" s="2">
         <v>433220086</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="2">
+    <row r="223" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A223" s="2">
         <v>433271689</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="2">
+    <row r="224" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A224" s="2">
         <v>433270086</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="2">
+    <row r="225" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A225" s="2">
         <v>433270182</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="2">
+    <row r="226" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A226" s="2">
         <v>433270184</v>
       </c>
     </row>
-    <row r="114" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="2">
+    <row r="227" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A227" s="2">
+        <v>433271022</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A228" s="2">
         <v>433271386</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="2">
+    <row r="229" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="2">
         <v>2438550252</v>
       </c>
     </row>
-    <row r="116" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="2">
+    <row r="230" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="2">
         <v>2438576253</v>
       </c>
     </row>
-    <row r="117" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="2">
+    <row r="231" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="2">
         <v>9430034281</v>
       </c>
     </row>

</xml_diff>